<commit_message>
Url encode parsing added for google maps url
</commit_message>
<xml_diff>
--- a/ModifiedClassList.xlsx
+++ b/ModifiedClassList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevesu/GIS School/GISCapstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE9A952-FF3F-884F-A6F4-858B4A061E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6680EF-48CA-3F47-87D3-2D5ACBEB3C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{2025F049-BA88-564F-B70D-48E09C4AC323}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{2025F049-BA88-564F-B70D-48E09C4AC323}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>Student ID#</t>
   </si>
@@ -69,6 +69,117 @@
   </si>
   <si>
     <t>T1Y 5T1</t>
+  </si>
+  <si>
+    <t>82821 SADDLEBROOK DRIVE NE</t>
+  </si>
+  <si>
+    <t>T3J 0M4</t>
+  </si>
+  <si>
+    <t>67 SADDLESTONE HEATH NE</t>
+  </si>
+  <si>
+    <t>Calgary</t>
+  </si>
+  <si>
+    <t>T3J 2B6</t>
+  </si>
+  <si>
+    <t>9033 46 ST NE</t>
+  </si>
+  <si>
+    <t>T3J 0Y9</t>
+  </si>
+  <si>
+    <t>156 CITADEL HILLS GREEN NW</t>
+  </si>
+  <si>
+    <t>T3G 3T5</t>
+  </si>
+  <si>
+    <t>700 MAHOGANY BLVD SE</t>
+  </si>
+  <si>
+    <t>T3M 1Y1</t>
+  </si>
+  <si>
+    <t>2436 39 ST SE</t>
+  </si>
+  <si>
+    <t>T2B 1A9</t>
+  </si>
+  <si>
+    <t>47 RANCH ESTATES DR NW</t>
+  </si>
+  <si>
+    <t>T3G 1J9</t>
+  </si>
+  <si>
+    <t>238 EDGEBURN LANE NW</t>
+  </si>
+  <si>
+    <t>T3A 4K1</t>
+  </si>
+  <si>
+    <t>247 ERIN MEADOW GREEN SE</t>
+  </si>
+  <si>
+    <t>T2B 3G3</t>
+  </si>
+  <si>
+    <t>613 40 ST NE</t>
+  </si>
+  <si>
+    <t>T2A 6S1</t>
+  </si>
+  <si>
+    <t>703-804 3 AVE SW</t>
+  </si>
+  <si>
+    <t>T2P 0G9</t>
+  </si>
+  <si>
+    <t>15 CEDARWOOD HILL SW</t>
+  </si>
+  <si>
+    <t>T2W 3H4</t>
+  </si>
+  <si>
+    <t>77 SADDLECREST GREEN</t>
+  </si>
+  <si>
+    <t>T3J 5N5</t>
+  </si>
+  <si>
+    <t>802 9A STREET NW</t>
+  </si>
+  <si>
+    <t>T2T 1S5</t>
+  </si>
+  <si>
+    <t>133 SADDLEFIELD PLACE NORTHEAST</t>
+  </si>
+  <si>
+    <t>T3J 4Z3</t>
+  </si>
+  <si>
+    <t>#717, 105 26 AVE SW</t>
+  </si>
+  <si>
+    <t>T2S 0M3</t>
+  </si>
+  <si>
+    <t>2A MILL VIEW WAY SW</t>
+  </si>
+  <si>
+    <t>T2Y 3E7</t>
+  </si>
+  <si>
+    <t>48 NOLANLAKE VIEW NW</t>
+  </si>
+  <si>
+    <t>T3R 0W3</t>
   </si>
 </sst>
 </file>
@@ -471,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DCC8928-5FBD-274D-99D0-37820336E52A}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,6 +641,312 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>115560.5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>105668.2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>95775.9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>85883.6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>75991.3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>66099</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>56206.7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>55555</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>36422.1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>26529.8</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>222777</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>222778</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>222779</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>222780</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>222781</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>222782</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>222783</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>222784</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>